<commit_message>
AUD Main Checks with ASX Future Codes
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD/AUD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD/AUD_MainChecks.xlsx
@@ -170,9 +170,6 @@
     <t>6AB</t>
   </si>
   <si>
-    <t>YBAM5</t>
-  </si>
-  <si>
     <t>Expiry-Value Date</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Shibor</t>
+  </si>
+  <si>
+    <t>YBAU5</t>
   </si>
 </sst>
 </file>
@@ -750,28 +750,28 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 17:12:59</v>
+        <v>Updated at 12:06:19</v>
         <stp/>
-        <stp>{3F86807B-6C96-43A1-9843-D760EF82B2E1}</stp>
-        <tr r="Q6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 17:19:32</v>
-        <stp/>
-        <stp>{858208FD-F141-4ED0-B57A-A790717C1E82}</stp>
+        <stp>{E523F481-6E52-4962-A946-9598A1B30562}</stp>
         <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 17:04:24</v>
+        <v>Updated at 12:06:19</v>
         <stp/>
-        <stp>{AE27E9C3-B4B4-45C4-A3A3-C874141F084B}</stp>
+        <stp>{37CD6EA1-90BF-4972-AE4F-803A76DB7722}</stp>
+        <tr r="Q7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:06:19</v>
+        <stp/>
+        <stp>{2B68A6F3-BF57-41F7-BBED-499C61B1B85B}</stp>
         <tr r="P7" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 17:04:24</v>
+        <v>Updated at 12:06:48</v>
         <stp/>
-        <stp>{1F1505C9-518F-4BB7-82D7-EEEDE56E41C2}</stp>
-        <tr r="Q7" s="2"/>
+        <stp>{CFD34DC6-F5A1-4C6D-B81B-BA2C454BB471}</stp>
+        <tr r="Q6" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1335,7 +1335,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>35</v>
@@ -1346,7 +1346,7 @@
         <v>6</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M4" s="13" t="s">
         <v>14</v>
@@ -1403,7 +1403,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>36</v>
@@ -1415,17 +1415,17 @@
         <v>TYcm1t</v>
       </c>
       <c r="L5" s="28">
-        <v>41992</v>
+        <v>42174</v>
       </c>
       <c r="M5" s="29">
-        <v>125.796875</v>
+        <v>126.65625</v>
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="29"/>
       <c r="P5" s="29"/>
       <c r="Q5" s="30" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 17:19:32</v>
+        <v>Updated at 12:06:19</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="U5" s="12" t="str">
         <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>1_52 / 1.5.0 / 1.5</v>
+        <v>1_57 / 1.6.0 / 1.6</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1474,7 +1474,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>36</v>
@@ -1482,20 +1482,20 @@
       <c r="I6" s="3"/>
       <c r="J6" s="21"/>
       <c r="K6" s="24" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="L6" s="25">
-        <v>42166</v>
+        <v>42257</v>
       </c>
       <c r="M6" s="31">
-        <v>97.28</v>
+        <v>97.89</v>
       </c>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
       <c r="Q6" s="32" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 17:12:59</v>
+        <v>Updated at 12:06:48</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="U6" s="12">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>903</v>
+        <v>963</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1544,7 +1544,7 @@
         <v>43</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>37</v>
@@ -1556,25 +1556,25 @@
         <v>AUDSM6AB10Y</v>
       </c>
       <c r="L7" s="25">
-        <v>41919</v>
+        <v>42171</v>
       </c>
       <c r="M7" s="34" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>3.7575/3.8175</v>
+        <v>3.3475/3.4075</v>
       </c>
       <c r="N7" s="31">
-        <v>3.7575000000000003</v>
+        <v>3.3475000000000001</v>
       </c>
       <c r="O7" s="31">
-        <v>3.8175000000000003</v>
+        <v>3.4075000000000002</v>
       </c>
       <c r="P7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 17:04:24</v>
+        <v>Updated at 12:06:19</v>
       </c>
       <c r="Q7" s="32" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 17:04:24</v>
+        <v>Updated at 12:06:19</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>13</v>
@@ -1606,7 +1606,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="38" t="s">
         <v>44</v>
@@ -1618,7 +1618,7 @@
         <v>30</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>36</v>
@@ -1676,7 +1676,7 @@
         <v>47</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>38</v>
@@ -1731,19 +1731,19 @@
         <v>16</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="47" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="46" t="s">
         <v>56</v>
-      </c>
-      <c r="G10" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="46" t="s">
-        <v>57</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
@@ -1751,20 +1751,20 @@
         <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
         <v>AudBBSW6M</v>
       </c>
-      <c r="L10" s="23" t="e">
-        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M10" s="33" t="e">
-        <f ca="1">_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NAME?</v>
+      <c r="L10" s="23">
+        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>42171</v>
+      </c>
+      <c r="M10" s="33">
+        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
       <c r="P10" s="33"/>
-      <c r="Q10" s="35" t="e">
-        <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
-        <v>#NAME?</v>
+      <c r="Q10" s="35" t="str">
+        <f>IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
+        <v/>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1799,7 +1799,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="47" t="s">
         <v>42</v>
@@ -1808,7 +1808,7 @@
         <v>43</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="46" t="s">
         <v>37</v>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="L11" s="25">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>41877</v>
+        <v>42171</v>
       </c>
       <c r="M11" s="26">
         <f>_xll.qlYieldTSDiscount(K11,L11)</f>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="L12" s="25">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>41877</v>
+        <v>42171</v>
       </c>
       <c r="M12" s="26">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="L13" s="25">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>41877</v>
+        <v>42171</v>
       </c>
       <c r="M13" s="26">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
@@ -1976,12 +1976,12 @@
         <v>1</v>
       </c>
       <c r="C14" s="39">
-        <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
-        <v>41899</v>
-      </c>
-      <c r="D14" s="6" t="e">
-        <f t="array" aca="1" ref="D14:D17" ca="1">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>#NAME?</v>
+        <f t="array" ref="C14:C17">_xll.qlASXNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
+        <v>42258</v>
+      </c>
+      <c r="D14" s="6" t="str">
+        <f t="array" ref="D14:D17">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlASXcode(FuturesDates)</f>
+        <v>YBAU5</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="L14" s="25">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>41877</v>
+        <v>42171</v>
       </c>
       <c r="M14" s="26">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
@@ -2036,11 +2036,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="40">
-        <v>41990</v>
-      </c>
-      <c r="D15" s="8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>42349</v>
+      </c>
+      <c r="D15" s="8" t="str">
+        <v>YBAZ5</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2054,7 +2053,7 @@
       </c>
       <c r="L15" s="25">
         <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>41877</v>
+        <v>42171</v>
       </c>
       <c r="M15" s="26">
         <f>_xll.qlYieldTSDiscount(K15,L15)</f>
@@ -2095,11 +2094,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="40">
-        <v>42081</v>
-      </c>
-      <c r="D16" s="8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>42440</v>
+      </c>
+      <c r="D16" s="8" t="str">
+        <v>YBAH6</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2142,11 +2140,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="41">
-        <v>42172</v>
-      </c>
-      <c r="D17" s="11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+        <v>42531</v>
+      </c>
+      <c r="D17" s="11" t="str">
+        <v>YBAM6</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -5364,7 +5361,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5384,12 +5381,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5409,7 +5406,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fixed bug: rolling futures adjusted in main checks
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD/AUD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD/AUD_MainChecks.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfondi\quantlib\QuantLibXL\Data2\XLS\AUD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="9600" windowHeight="12015"/>
   </bookViews>
@@ -19,12 +24,12 @@
     <definedName name="TenYearsBondFutures">MainChecks!$C$4:$C$6</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>ObjectID</t>
   </si>
@@ -195,16 +200,13 @@
   </si>
   <si>
     <t>Shibor</t>
-  </si>
-  <si>
-    <t>YBAU5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
     <numFmt numFmtId="166" formatCode="ddd\,\ dd\-mmm\-yyyy"/>
@@ -213,7 +215,6 @@
     <numFmt numFmtId="169" formatCode="0.0000"/>
     <numFmt numFmtId="170" formatCode="0.000000000"/>
     <numFmt numFmtId="171" formatCode="ddd\,\ dd\-mmm\-yyyy\ hh:mm:ss"/>
-    <numFmt numFmtId="172" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -639,9 +640,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -741,41 +742,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 12:06:19</v>
-        <stp/>
-        <stp>{E523F481-6E52-4962-A946-9598A1B30562}</stp>
-        <tr r="Q5" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:06:19</v>
-        <stp/>
-        <stp>{37CD6EA1-90BF-4972-AE4F-803A76DB7722}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:06:19</v>
-        <stp/>
-        <stp>{2B68A6F3-BF57-41F7-BBED-499C61B1B85B}</stp>
-        <tr r="P7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:06:48</v>
-        <stp/>
-        <stp>{CFD34DC6-F5A1-4C6D-B81B-BA2C454BB471}</stp>
-        <tr r="Q6" s="2"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -814,7 +785,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -822,6 +793,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -855,7 +840,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -863,6 +848,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -916,7 +915,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,7 +950,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1415,17 +1414,17 @@
         <v>TYcm1t</v>
       </c>
       <c r="L5" s="28">
-        <v>42174</v>
+        <v>41992</v>
       </c>
       <c r="M5" s="29">
-        <v>126.65625</v>
+        <v>125.796875</v>
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="29"/>
       <c r="P5" s="29"/>
-      <c r="Q5" s="30" t="str">
-        <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 12:06:19</v>
+      <c r="Q5" s="30" t="e">
+        <f ca="1">_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1434,9 +1433,9 @@
       <c r="T5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="12" t="str">
-        <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>1_57 / 1.6.0 / 1.6</v>
+      <c r="U5" s="12" t="e">
+        <f ca="1">_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
+        <v>#NAME?</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1481,21 +1480,22 @@
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="21"/>
-      <c r="K6" s="24" t="s">
-        <v>57</v>
+      <c r="K6" s="24" t="e">
+        <f ca="1">D14</f>
+        <v>#NAME?</v>
       </c>
       <c r="L6" s="25">
-        <v>42257</v>
+        <v>42166</v>
       </c>
       <c r="M6" s="31">
-        <v>97.89</v>
+        <v>97.28</v>
       </c>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
-      <c r="Q6" s="32" t="str">
-        <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 12:06:48</v>
+      <c r="Q6" s="32" t="e">
+        <f ca="1">_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1504,9 +1504,9 @@
       <c r="T6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="12">
-        <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>963</v>
+      <c r="U6" s="12" t="e">
+        <f ca="1">_xll.ohRepositoryObjectCount(Trigger)</f>
+        <v>#NAME?</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1556,25 +1556,25 @@
         <v>AUDSM6AB10Y</v>
       </c>
       <c r="L7" s="25">
-        <v>42171</v>
+        <v>41919</v>
       </c>
       <c r="M7" s="34" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>3.3475/3.4075</v>
+        <v>3.7575/3.8175</v>
       </c>
       <c r="N7" s="31">
-        <v>3.3475000000000001</v>
+        <v>3.7575000000000003</v>
       </c>
       <c r="O7" s="31">
-        <v>3.4075000000000002</v>
-      </c>
-      <c r="P7" s="31" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 12:06:19</v>
-      </c>
-      <c r="Q7" s="32" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 12:06:19</v>
+        <v>3.8175000000000003</v>
+      </c>
+      <c r="P7" s="31" t="e">
+        <f ca="1">_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q7" s="32" t="e">
+        <f ca="1">_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>13</v>
@@ -1751,20 +1751,20 @@
         <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
         <v>AudBBSW6M</v>
       </c>
-      <c r="L10" s="23">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>42171</v>
-      </c>
-      <c r="M10" s="33">
-        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>2.2599999999999999E-2</v>
+      <c r="L10" s="23" t="e">
+        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M10" s="33" t="e">
+        <f ca="1">_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
       <c r="P10" s="33"/>
-      <c r="Q10" s="35" t="str">
-        <f>IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
-        <v/>
+      <c r="Q10" s="35" t="e">
+        <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
+        <v>#NAME?</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1819,20 +1819,20 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>AUDSTD</v>
       </c>
-      <c r="L11" s="25">
-        <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>42171</v>
-      </c>
-      <c r="M11" s="26">
-        <f>_xll.qlYieldTSDiscount(K11,L11)</f>
-        <v>1</v>
+      <c r="L11" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M11" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K11,L11)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
       <c r="P11" s="26"/>
-      <c r="Q11" s="36" t="str">
-        <f>IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
-        <v/>
+      <c r="Q11" s="36" t="e">
+        <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
+        <v>#NAME?</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>13</v>
@@ -1881,20 +1881,20 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>AUDON</v>
       </c>
-      <c r="L12" s="25">
-        <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>42171</v>
-      </c>
-      <c r="M12" s="26">
-        <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>1</v>
+      <c r="L12" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M12" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K12,L12)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
       <c r="P12" s="26"/>
-      <c r="Q12" s="37" t="str">
-        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v/>
+      <c r="Q12" s="37" t="e">
+        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v>#NAME?</v>
       </c>
       <c r="R12" s="8" t="s">
         <v>13</v>
@@ -1933,20 +1933,20 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>AUD1M</v>
       </c>
-      <c r="L13" s="25">
-        <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>42171</v>
-      </c>
-      <c r="M13" s="26">
-        <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>1</v>
+      <c r="L13" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M13" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K13,L13)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N13" s="26"/>
       <c r="O13" s="26"/>
       <c r="P13" s="26"/>
-      <c r="Q13" s="37" t="str">
-        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v/>
+      <c r="Q13" s="37" t="e">
+        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <v>#NAME?</v>
       </c>
       <c r="R13" s="8" t="s">
         <v>13</v>
@@ -1975,13 +1975,13 @@
       <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="39">
-        <f t="array" ref="C14:C17">_xll.qlASXNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
-        <v>42258</v>
-      </c>
-      <c r="D14" s="6" t="str">
-        <f t="array" ref="D14:D17">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlASXcode(FuturesDates)</f>
-        <v>YBAU5</v>
+      <c r="C14" s="39" t="e">
+        <f t="array" aca="1" ref="C14:C17" ca="1">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D14" s="6" t="e">
+        <f t="array" aca="1" ref="D14:D17" ca="1">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
+        <v>#NAME?</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1993,20 +1993,20 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>AUD3M</v>
       </c>
-      <c r="L14" s="25">
-        <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>42171</v>
-      </c>
-      <c r="M14" s="26">
-        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>1</v>
+      <c r="L14" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M14" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K14,L14)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="26"/>
-      <c r="Q14" s="37" t="str">
-        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v/>
+      <c r="Q14" s="37" t="e">
+        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v>#NAME?</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>13</v>
@@ -2035,11 +2035,13 @@
       <c r="B15" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="40">
-        <v>42349</v>
-      </c>
-      <c r="D15" s="8" t="str">
-        <v>YBAZ5</v>
+      <c r="C15" s="40" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D15" s="8" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2051,20 +2053,20 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>AUD6M</v>
       </c>
-      <c r="L15" s="25">
-        <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>42171</v>
-      </c>
-      <c r="M15" s="26">
-        <f>_xll.qlYieldTSDiscount(K15,L15)</f>
-        <v>1</v>
+      <c r="L15" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M15" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K15,L15)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
       <c r="P15" s="26"/>
-      <c r="Q15" s="37" t="str">
-        <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v/>
+      <c r="Q15" s="37" t="e">
+        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
+        <v>#NAME?</v>
       </c>
       <c r="R15" s="8" t="s">
         <v>13</v>
@@ -2093,11 +2095,13 @@
       <c r="B16" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="40">
-        <v>42440</v>
-      </c>
-      <c r="D16" s="8" t="str">
-        <v>YBAH6</v>
+      <c r="C16" s="40" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D16" s="8" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2139,11 +2143,13 @@
       <c r="B17" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="41">
-        <v>42531</v>
-      </c>
-      <c r="D17" s="11" t="str">
-        <v>YBAM6</v>
+      <c r="C17" s="41" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D17" s="11" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -5345,12 +5351,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4">
       <formula1>"EUR,USD,GBP,JPY,CHF,AUD,CNY,CNH,HKD"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6">
-      <formula1>IMMFutures</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>